<commit_message>
1. DoPlaySheet -> RVL.DoPlayTest to have cleaner report 2. TestPrepare with navigation to site according to Config.xlsx
</commit_message>
<xml_diff>
--- a/OpenMRS_DDT/CheckDashboardTiles/Main.rvl.xlsx
+++ b/OpenMRS_DDT/CheckDashboardTiles/Main.rvl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="107">
   <si>
     <t>Flow</t>
   </si>
@@ -331,6 +331,12 @@
   </si>
   <si>
     <t>Message</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Data1</t>
   </si>
 </sst>
 </file>
@@ -662,7 +668,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -795,6 +801,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -840,7 +852,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0"/>
@@ -861,6 +873,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="true"/>
@@ -1262,7 +1280,7 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -1423,7 +1441,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
         <v>99</v>
@@ -1466,7 +1484,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -1485,7 +1503,7 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>106</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>

</xml_diff>